<commit_message>
Upload some documentation to the repository
</commit_message>
<xml_diff>
--- a/Database Mapping.xlsx
+++ b/Database Mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -29,21 +29,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ManagerID</t>
-  </si>
-  <si>
-    <t>StartDate</t>
-  </si>
-  <si>
-    <t>AccruedPTO</t>
-  </si>
-  <si>
-    <t>AvailableSick</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -56,25 +41,97 @@
     <t>Status</t>
   </si>
   <si>
-    <t>EndDate</t>
-  </si>
-  <si>
     <t>PTORequested</t>
   </si>
   <si>
-    <t>SickRequested</t>
-  </si>
-  <si>
-    <t>UsedPTO</t>
-  </si>
-  <si>
-    <t>UsedSick</t>
-  </si>
-  <si>
-    <t>UsedUnpaid</t>
-  </si>
-  <si>
-    <t>UnpaidRequested</t>
+    <t>TimeOffId</t>
+  </si>
+  <si>
+    <t>TimeClockID</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>sickRequested</t>
+  </si>
+  <si>
+    <t>unpaidRequested</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>managerid</t>
+  </si>
+  <si>
+    <t>accruedPTO</t>
+  </si>
+  <si>
+    <t>usedPTO</t>
+  </si>
+  <si>
+    <t>availableSick</t>
+  </si>
+  <si>
+    <t>usedSick</t>
+  </si>
+  <si>
+    <t>availableFloater</t>
+  </si>
+  <si>
+    <t>usedFloater</t>
+  </si>
+  <si>
+    <t>usedUnpaid</t>
+  </si>
+  <si>
+    <t>Roger West</t>
+  </si>
+  <si>
+    <t>Jack Ma</t>
+  </si>
+  <si>
+    <t>jack123</t>
+  </si>
+  <si>
+    <t>roger123</t>
+  </si>
+  <si>
+    <t>David Faulkner</t>
+  </si>
+  <si>
+    <t>david123</t>
+  </si>
+  <si>
+    <t>Bryan Mapula</t>
+  </si>
+  <si>
+    <t>bryan123</t>
+  </si>
+  <si>
+    <t>john123</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Jane</t>
   </si>
 </sst>
 </file>
@@ -392,82 +449,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>101</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>101</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>16</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>101</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>104</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -477,40 +763,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>